<commit_message>
procedimientos actualizados *UDP_Acce_tbUsuario_Insert     (tocado en la base) *SDP_tbEmpleado_Select   (tocado en la base) *SDP_Gral_tbEmpleado_Select  (tocado en la base)
--controlador de usuario
*en Create se modifico un parametro a "true" que se manda al procedimiento

--la vista Create de usuario
*se modifico un nombre de procedimiento complejo de "SDP_tbEmpleado_Select_Result" a "SDP_tbEmpleado_Select_Result1"

la vista parcial de _BuscarEmpleado
*se cambio el nombre del procedimiento complejo de "SDP_tbEmpleado_Select_Result" a "SDP_tbEmpleado_Select_Result1"
*en los campos se cambiarion los campos por item.per_Nombres,item.per_Apellidos,item.per_CorreoElectronico
</commit_message>
<xml_diff>
--- a/ERP_GMEDINA/Downloadable files/ArchivoEmpleados.xlsx
+++ b/ERP_GMEDINA/Downloadable files/ArchivoEmpleados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab 1.DESKTOP-7RAR2G4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab 1.DESKTOP-UPVD3NF\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B69FBD-B6ED-4298-A566-D3241E5CB9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF9AA33-8EA8-43E7-918F-F6B056694F45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArchivoEmpleados" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="107">
   <si>
     <t>FAVOR LLENAR UNICAMENTE LA INFORMACION SOLICITADA, NO CAMBIAR NINGUNA CONFIGURACION DE ESTE DOCUMENTO</t>
   </si>
@@ -31,10 +31,10 @@
     <t>Hondureña</t>
   </si>
   <si>
-    <t>Area Abierta</t>
+    <t>Testing</t>
   </si>
   <si>
-    <t>Departamento de IT</t>
+    <t>IT</t>
   </si>
   <si>
     <t>Matutina</t>
@@ -58,7 +58,7 @@
     <t>Brasileña</t>
   </si>
   <si>
-    <t>Vendedores</t>
+    <t>Prueba</t>
   </si>
   <si>
     <t>Vespertina</t>
@@ -79,7 +79,10 @@
     <t>Chilena</t>
   </si>
   <si>
-    <t>IT</t>
+    <t>Comunicacion y diseño</t>
+  </si>
+  <si>
+    <t>informaticas</t>
   </si>
   <si>
     <t>Nocturna</t>
@@ -166,10 +169,7 @@
     <t>Colombiana</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Prueba</t>
+    <t>dba</t>
   </si>
   <si>
     <t>Fin de semana</t>
@@ -181,28 +181,28 @@
     <t>Tarjeta de Crédito</t>
   </si>
   <si>
+    <t>Libra esterlina</t>
+  </si>
+  <si>
     <t>Ingeniero en Sistemas</t>
   </si>
   <si>
     <t>Costarricense</t>
   </si>
   <si>
-    <t>informaticas</t>
+    <t>Vendedores</t>
   </si>
   <si>
     <t>Transferencia Bancaria</t>
+  </si>
+  <si>
+    <t>Won</t>
   </si>
   <si>
     <t>Programador</t>
   </si>
   <si>
     <t>Cubana</t>
-  </si>
-  <si>
-    <t>Comunicacion y diseño</t>
-  </si>
-  <si>
-    <t>dba</t>
   </si>
   <si>
     <t>Planilla Gerentes</t>
@@ -319,34 +319,28 @@
     <t>Coreana</t>
   </si>
   <si>
-    <t>0501-2001-07846</t>
+    <t>M</t>
   </si>
   <si>
-    <t>Gabriela Yessenia</t>
+    <t>COL.PAZ</t>
   </si>
   <si>
-    <t>Zepeda Chavarria</t>
+    <t>david@gmail.com</t>
   </si>
   <si>
-    <t>F</t>
+    <t>C</t>
   </si>
   <si>
-    <t>Col. Villa Ernestina</t>
+    <t>AB+</t>
   </si>
   <si>
-    <t>2509-9402</t>
+    <t>081242004245100</t>
   </si>
   <si>
-    <t>chavarriag156@gmail.com</t>
+    <t>Jose1 David3</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>O+</t>
-  </si>
-  <si>
-    <t>051428462</t>
+    <t>Zapata3</t>
   </si>
 </sst>
 </file>
@@ -358,7 +352,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -377,6 +371,10 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -749,14 +747,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:MH10000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="3" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
@@ -765,9 +764,11 @@
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="13.5703125" customWidth="1"/>
     <col min="20" max="21" width="15.7109375" customWidth="1"/>
     <col min="22" max="22" width="13.140625" customWidth="1"/>
@@ -1032,99 +1033,99 @@
         <v>18</v>
       </c>
       <c r="MC3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="MD3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="ME3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="MF3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="MG3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="MH3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:346">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="MA4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="MB4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="MC4" s="3" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="MD4" s="3" t="s">
         <v>49</v>
@@ -1138,109 +1139,44 @@
       <c r="MG4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:346">
-      <c r="A5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="2">
-        <v>36854</v>
-      </c>
-      <c r="E5">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L5" t="s">
-        <v>107</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5" s="2">
-        <v>42865</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="U5" s="5">
-        <v>50000</v>
-      </c>
-      <c r="V5" t="s">
-        <v>8</v>
-      </c>
-      <c r="MA5" s="3" t="s">
+      <c r="MH4" t="s">
         <v>53</v>
       </c>
-      <c r="MB5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:346">
+      <c r="A5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="J5" s="7"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="5"/>
+      <c r="MA5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="MC5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="MD5" s="3" t="s">
+      <c r="MB5" s="3" t="s">
         <v>55</v>
       </c>
       <c r="MF5" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="MG5" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="MH5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:346">
       <c r="A6" s="1"/>
       <c r="D6" s="2"/>
+      <c r="J6" s="7"/>
       <c r="S6" s="2"/>
       <c r="T6" s="4"/>
       <c r="U6" s="5"/>
       <c r="MA6" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="MB6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="MC6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="MD6" s="3" t="s">
         <v>60</v>
       </c>
       <c r="MF6" t="s">
@@ -1251,19 +1187,77 @@
       </c>
     </row>
     <row r="7" spans="1:346">
-      <c r="A7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="5"/>
+      <c r="A7" s="1">
+        <v>89685245263254</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44179</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>98465751</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="2">
+        <v>44177</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="U7" s="5">
+        <v>12000</v>
+      </c>
+      <c r="V7" t="s">
+        <v>24</v>
+      </c>
       <c r="MA7" s="3" t="s">
         <v>63</v>
       </c>
       <c r="MB7" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="MC7" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="MF7" t="s">
         <v>65</v>
@@ -1288,7 +1282,7 @@
         <v>69</v>
       </c>
       <c r="MG8" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:346">
@@ -1307,7 +1301,7 @@
         <v>72</v>
       </c>
       <c r="MG9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:346">
@@ -44329,6 +44323,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:V3"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="11">
     <dataValidation type="list" sqref="F5:F1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"F,M"</formula1>
@@ -44346,10 +44341,10 @@
       <formula1>$MA$1:$MA$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N5:N1000" xr:uid="{00000000-0002-0000-0000-000005000000}">
-      <formula1>$MC$1:$MC$7</formula1>
+      <formula1>$MC$1:$MC$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O5:O1000" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$MD$1:$MD$6</formula1>
+      <formula1>$MD$1:$MD$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P5:P1000" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>$ME$1:$ME$4</formula1>
@@ -44365,7 +44360,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J5" r:id="rId1" xr:uid="{04073A2E-CEB8-471D-88B5-E3745BF01B0A}"/>
+    <hyperlink ref="J6:J7" r:id="rId1" display="david@gmail.com" xr:uid="{65F9F30A-2178-472A-B7C9-2A43C100E444}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>